<commit_message>
headless browser and more fixes
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4499460C-0437-45B7-9ACD-DC79B3892340}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467F1145-30AB-4BFF-A90F-92AE003815ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="25860" windowHeight="11715" xr2:uid="{0B981B8D-C0FE-4817-BF65-35702E84E83A}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TrialsJournal" sheetId="6" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Google Scholar" sheetId="1" r:id="rId3"/>
+    <sheet name="PubMed" sheetId="4" r:id="rId4"/>
+    <sheet name="zorgkaartnederland.nl(rating)" sheetId="3" r:id="rId5"/>
+    <sheet name="PubFacts" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,104 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+  <si>
+    <t>HCP Full Name</t>
+  </si>
+  <si>
+    <t>Found Name</t>
+  </si>
+  <si>
+    <t>Image URL</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Affiliation</t>
+  </si>
+  <si>
+    <t>Research Area</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>H-index</t>
+  </si>
+  <si>
+    <t>i10-index</t>
+  </si>
+  <si>
+    <t>Article List</t>
+  </si>
+  <si>
+    <t>CoAuthors</t>
+  </si>
+  <si>
+    <t>IsExactMatch(100% match)</t>
+  </si>
+  <si>
+    <t>Source URL</t>
+  </si>
+  <si>
+    <t>Google Scholar(Found/Not Found)</t>
+  </si>
+  <si>
+    <t>Google Scholar match %(if Found)</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Workplace</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>zorgkaartnederland.nl-rating(Found/Not Found)</t>
+  </si>
+  <si>
+    <t>zorgkaartnederland.nl-rating match (if found)</t>
+  </si>
+  <si>
+    <t>PubMed(Found/Not Found)</t>
+  </si>
+  <si>
+    <t>PubMed Match %(if Found)</t>
+  </si>
+  <si>
+    <t>PubFacts(Found/Not Found)</t>
+  </si>
+  <si>
+    <t>PubFacts %(if Found)</t>
+  </si>
+  <si>
+    <t>TrialsJournal (Found / Not Found)</t>
+  </si>
+  <si>
+    <t>Trails Journal %(if Found)</t>
+  </si>
+  <si>
+    <t>NOT FOUND</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,13 +129,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,7 +205,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -103,7 +217,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -150,23 +264,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -202,23 +299,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -370,13 +450,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC161F3-D2DD-4434-9A51-DB5A54236EFF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F312B4-F879-46C4-BFD1-C8DFD460DABB}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF5F6C8-11F1-43BC-A2FB-C4DB22B2B36E}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E456C4A0-5EB5-49A7-9F47-309DF36F7FEF}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A6AA72-B163-4BD4-AF47-72380F3D6597}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465DB926-DD3C-49E9-BE5A-2AE6D457718B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>